<commit_message>
Initial upload for Korean
Apply v3.1.1
https://siriusstars.tistory.com/18
</commit_message>
<xml_diff>
--- a/jyx2/Assets/Mods/JYX2/Configs/场景.xlsx
+++ b/jyx2/Assets/Mods/JYX2/Configs/场景.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\jynew\jyx2\Assets\Mods\jytest\Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\jynew-20230510\jyx2\Assets\Mods\JYX2\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C18A68-72CD-4A51-BD04-4EAA2BD68D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7C821-795F-445B-96CF-21D45DD8088D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1210" yWindow="6230" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11085" yWindow="1875" windowWidth="25350" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="204">
   <si>
     <t>Id</t>
   </si>
@@ -133,36 +133,21 @@
     </r>
   </si>
   <si>
-    <t>胡斐居</t>
-  </si>
-  <si>
     <t>00_hufeiju</t>
   </si>
   <si>
     <t>Leave:1000</t>
   </si>
   <si>
-    <t>河洛客栈</t>
-  </si>
-  <si>
     <t>01_heluokezhan</t>
   </si>
   <si>
-    <t>云鹤崖</t>
-  </si>
-  <si>
     <t>02_yunheya</t>
   </si>
   <si>
-    <t>有间客栈</t>
-  </si>
-  <si>
     <t>03_youjiankezhan</t>
   </si>
   <si>
-    <t>昆仑仙境</t>
-  </si>
-  <si>
     <t>04_kunlunxianjing</t>
   </si>
   <si>
@@ -172,635 +157,565 @@
     <t>POINTLIGHT</t>
   </si>
   <si>
+    <t>05_shandong</t>
+  </si>
+  <si>
+    <t>06_beichouju</t>
+  </si>
+  <si>
+    <t>07_shandong</t>
+  </si>
+  <si>
+    <t>08_dalunsi</t>
+  </si>
+  <si>
+    <t>09_chengkunju</t>
+  </si>
+  <si>
+    <t>10_shandong</t>
+  </si>
+  <si>
+    <t>11_guangmingding</t>
+  </si>
+  <si>
+    <t>12_mingjiaofenduo</t>
+  </si>
+  <si>
+    <t>Leave:1000,Leave2:13</t>
+  </si>
+  <si>
+    <t>13_mingjiaodidao</t>
+  </si>
+  <si>
+    <t>Leave:12</t>
+  </si>
+  <si>
+    <t>14_gaochangmigong</t>
+  </si>
+  <si>
+    <t>Leave:15</t>
+  </si>
+  <si>
+    <t>15_shamofeixu</t>
+  </si>
+  <si>
+    <t>Leave:1000,Leave2:14</t>
+  </si>
+  <si>
+    <t>16_jinlunsi</t>
+  </si>
+  <si>
+    <t>17_huizubuluo</t>
+  </si>
+  <si>
+    <t>18_gumu</t>
+  </si>
+  <si>
+    <t>19_chongyanggong</t>
+  </si>
+  <si>
+    <t>20_baihuagu</t>
+  </si>
+  <si>
+    <t>21_heilongtan</t>
+  </si>
+  <si>
+    <t>NONAVAGENT</t>
+  </si>
+  <si>
+    <t>22_jueqinggu</t>
+  </si>
+  <si>
+    <t>23_hongqigongju</t>
+  </si>
+  <si>
+    <t>24_miaorenfengju</t>
+  </si>
+  <si>
+    <t>25_wudaodahui</t>
+  </si>
+  <si>
+    <t>26_heimuya</t>
+  </si>
+  <si>
+    <t>27_songshanpai</t>
+  </si>
+  <si>
+    <t>28_shaolinsi</t>
+  </si>
+  <si>
+    <t>29_taishanpai</t>
+  </si>
+  <si>
+    <t>30_pingyizhiju</t>
+  </si>
+  <si>
+    <t>31_hengshanpai</t>
+  </si>
+  <si>
+    <t>32_haibianxiaowu</t>
+  </si>
+  <si>
+    <t>33_emeipai</t>
+  </si>
+  <si>
+    <t>34_kongtongpai</t>
+  </si>
+  <si>
+    <t>35_xingxiuhai</t>
+  </si>
+  <si>
+    <t>36_qingchengpai</t>
+  </si>
+  <si>
+    <t>37_wudujiao</t>
+  </si>
+  <si>
+    <t>38_motianya</t>
+  </si>
+  <si>
+    <t>39_lingxiaocheng</t>
+  </si>
+  <si>
+    <t>40_yuelaikezhan</t>
+  </si>
+  <si>
+    <t>41_shandong</t>
+  </si>
+  <si>
+    <t>42_wuliangshandong</t>
+  </si>
+  <si>
+    <t>43_wudangpai</t>
+  </si>
+  <si>
+    <t>44_hudiegu</t>
+  </si>
+  <si>
+    <t>45_chengyingju</t>
+  </si>
+  <si>
+    <t>46_jinsheshandong</t>
+  </si>
+  <si>
+    <t>47_yidengju</t>
+  </si>
+  <si>
+    <t>48_tiezhangshan</t>
+  </si>
+  <si>
+    <t>49_yaowangzhuang</t>
+  </si>
+  <si>
+    <t>50_yanjiju</t>
+  </si>
+  <si>
+    <t>51_gaibang</t>
+  </si>
+  <si>
+    <t>52_yanziwu</t>
+  </si>
+  <si>
+    <t>53_leigushan</t>
+  </si>
+  <si>
+    <t>54_xuemuhuaju</t>
+  </si>
+  <si>
+    <t>55_meizhuang</t>
+  </si>
+  <si>
+    <t>Leave:1000,Leave2:82</t>
+  </si>
+  <si>
+    <t>56_fuweibiaoju</t>
+  </si>
+  <si>
+    <t>57_huashanpai</t>
+  </si>
+  <si>
+    <t>58_hengshanpai</t>
+  </si>
+  <si>
+    <t>59_tianboguangju</t>
+  </si>
+  <si>
+    <t>60_longmenkezhan</t>
+  </si>
+  <si>
+    <t>61_gaoshengkezhan</t>
+  </si>
+  <si>
+    <t>62_pomiao</t>
+  </si>
+  <si>
+    <t>63_tianningsi</t>
+  </si>
+  <si>
+    <t>64_nanxianju</t>
+  </si>
+  <si>
+    <t>65_shandong</t>
+  </si>
+  <si>
+    <t>66_shandong</t>
+  </si>
+  <si>
+    <t>67_shandong</t>
+  </si>
+  <si>
+    <t>Leave:1000,Leave2:4</t>
+  </si>
+  <si>
+    <t>68_kunlunpai</t>
+  </si>
+  <si>
+    <t>69_baituoshan</t>
+  </si>
+  <si>
+    <t>70_xiaoxiamiju</t>
+  </si>
+  <si>
+    <t>START:0</t>
+  </si>
+  <si>
+    <t>71_shenlongjiao</t>
+  </si>
+  <si>
+    <t>72_binghuodao</t>
+  </si>
+  <si>
+    <t>73_lingshedao</t>
+  </si>
+  <si>
+    <t>74_xiakedao</t>
+  </si>
+  <si>
+    <t>75_taohuadao</t>
+  </si>
+  <si>
+    <t>76_pilitang</t>
+  </si>
+  <si>
+    <t>Leave:1000,Leave2:83</t>
+  </si>
+  <si>
+    <t>77_wanedao</t>
+  </si>
+  <si>
+    <t>78_bonidao</t>
+  </si>
+  <si>
+    <t>79_shandong</t>
+  </si>
+  <si>
+    <t>80_jueqinggudi</t>
+  </si>
+  <si>
+    <t>81_siguoya</t>
+  </si>
+  <si>
+    <t>82_meizhuangdilao</t>
+  </si>
+  <si>
+    <t>Leave:55</t>
+  </si>
+  <si>
+    <t>83_shengtang</t>
+  </si>
+  <si>
+    <t>Leave:76</t>
+  </si>
+  <si>
+    <t>WORLDMAP</t>
+  </si>
+  <si>
+    <t>1000_daditu</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>LuaConfigGen</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>L_number</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>L_string</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>호비거처</t>
+  </si>
+  <si>
+    <t>하락객잔</t>
+  </si>
+  <si>
+    <t>운학애</t>
+  </si>
+  <si>
+    <t>유간객잔</t>
+  </si>
+  <si>
+    <t>곤륜선경</t>
+  </si>
+  <si>
+    <t>북추거처</t>
+  </si>
+  <si>
+    <t>신조동굴</t>
+  </si>
+  <si>
+    <t>대륜사</t>
+  </si>
+  <si>
+    <t>성곤거처</t>
+  </si>
+  <si>
+    <t>거미동굴</t>
+  </si>
+  <si>
+    <t>광명정</t>
+  </si>
+  <si>
+    <t>명교분타</t>
+  </si>
+  <si>
+    <t>명교갱도</t>
+  </si>
+  <si>
+    <t>고창미궁</t>
+  </si>
+  <si>
+    <t>사막폐허</t>
+  </si>
+  <si>
+    <t>금륜사</t>
+  </si>
+  <si>
+    <t>회족부락</t>
+  </si>
+  <si>
+    <t>고묘</t>
+  </si>
+  <si>
+    <t>중양궁</t>
+  </si>
+  <si>
+    <t>백화곡</t>
+  </si>
+  <si>
+    <t>흑룡담</t>
+  </si>
+  <si>
+    <t>절정곡</t>
+  </si>
+  <si>
+    <t>홍칠공거처</t>
+  </si>
+  <si>
+    <t>묘인봉거처</t>
+  </si>
+  <si>
+    <t>화산논검</t>
+  </si>
+  <si>
+    <t>흑목애</t>
+  </si>
+  <si>
+    <t>숭산파</t>
+  </si>
+  <si>
+    <t>소림사</t>
+  </si>
+  <si>
+    <t>태산파</t>
+  </si>
+  <si>
+    <t>평일지거처</t>
+  </si>
+  <si>
+    <t>항산파</t>
+  </si>
+  <si>
+    <t>해변초가</t>
+  </si>
+  <si>
+    <t>아미파</t>
+  </si>
+  <si>
+    <t>공동파</t>
+  </si>
+  <si>
+    <t>청성파</t>
+  </si>
+  <si>
+    <t>오독교</t>
+  </si>
+  <si>
+    <t>마천애</t>
+  </si>
+  <si>
+    <t>능소성</t>
+  </si>
+  <si>
+    <t>열래(악래)객잔</t>
+  </si>
+  <si>
+    <t>신비동굴</t>
+  </si>
+  <si>
+    <t>무량동굴</t>
+  </si>
+  <si>
+    <t>무당파</t>
+  </si>
+  <si>
+    <t>호접곡</t>
+  </si>
+  <si>
+    <t>정영거처</t>
+  </si>
+  <si>
+    <t>금사동굴</t>
+  </si>
+  <si>
+    <t>일등거처</t>
+  </si>
+  <si>
+    <t>철장산</t>
+  </si>
+  <si>
+    <t>약왕장</t>
+  </si>
+  <si>
+    <t>염기거처</t>
+  </si>
+  <si>
+    <t>개방</t>
+  </si>
+  <si>
+    <t>연자오</t>
+  </si>
+  <si>
+    <t>뇌고산</t>
+  </si>
+  <si>
+    <t>매장</t>
+  </si>
+  <si>
+    <t>복위표국</t>
+  </si>
+  <si>
+    <t>화산파</t>
+  </si>
+  <si>
+    <t>형산파</t>
+  </si>
+  <si>
+    <t>전백광거처</t>
+  </si>
+  <si>
+    <t>용문객잔</t>
+  </si>
+  <si>
+    <t>고승객잔</t>
+  </si>
+  <si>
+    <t>파묘</t>
+  </si>
+  <si>
+    <t>천녕사</t>
+  </si>
+  <si>
+    <t>남현거처</t>
+  </si>
+  <si>
+    <t>당시동굴</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>빙잠동굴</t>
+  </si>
+  <si>
+    <t>곤륜파</t>
+  </si>
+  <si>
+    <t>백타산</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>闯王山洞</t>
+      <t>小</t>
     </r>
-  </si>
-  <si>
-    <t>05_shandong</t>
-  </si>
-  <si>
-    <t>北丑居</t>
-  </si>
-  <si>
-    <t>06_beichouju</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>神雕山洞</t>
-    </r>
-  </si>
-  <si>
-    <t>07_shandong</t>
-  </si>
-  <si>
-    <t>大轮寺</t>
-  </si>
-  <si>
-    <t>08_dalunsi</t>
-  </si>
-  <si>
-    <t>成昆居</t>
-  </si>
-  <si>
-    <t>09_chengkunju</t>
-  </si>
-  <si>
-    <t>蜘蛛山洞</t>
-  </si>
-  <si>
-    <t>10_shandong</t>
-  </si>
-  <si>
-    <t>光明顶</t>
-  </si>
-  <si>
-    <t>11_guangmingding</t>
-  </si>
-  <si>
-    <t>明教分舵</t>
-  </si>
-  <si>
-    <t>12_mingjiaofenduo</t>
-  </si>
-  <si>
-    <t>Leave:1000,Leave2:13</t>
-  </si>
-  <si>
-    <t>明教地道</t>
-  </si>
-  <si>
-    <t>13_mingjiaodidao</t>
-  </si>
-  <si>
-    <t>Leave:12</t>
-  </si>
-  <si>
-    <t>高昌迷宫</t>
-  </si>
-  <si>
-    <t>14_gaochangmigong</t>
-  </si>
-  <si>
-    <t>Leave:15</t>
-  </si>
-  <si>
-    <t>沙漠废墟</t>
-  </si>
-  <si>
-    <t>15_shamofeixu</t>
-  </si>
-  <si>
-    <t>Leave:1000,Leave2:14</t>
-  </si>
-  <si>
-    <t>金轮寺</t>
-  </si>
-  <si>
-    <t>16_jinlunsi</t>
-  </si>
-  <si>
-    <t>回族部落</t>
-  </si>
-  <si>
-    <t>17_huizubuluo</t>
-  </si>
-  <si>
-    <t>古墓</t>
-  </si>
-  <si>
-    <t>18_gumu</t>
-  </si>
-  <si>
-    <t>重阳宫</t>
-  </si>
-  <si>
-    <t>19_chongyanggong</t>
-  </si>
-  <si>
-    <t>百花谷</t>
-  </si>
-  <si>
-    <t>20_baihuagu</t>
-  </si>
-  <si>
-    <t>黑龙潭</t>
-  </si>
-  <si>
-    <t>21_heilongtan</t>
-  </si>
-  <si>
-    <t>NONAVAGENT</t>
-  </si>
-  <si>
-    <t>绝情谷</t>
-  </si>
-  <si>
-    <t>22_jueqinggu</t>
-  </si>
-  <si>
-    <t>洪七公居</t>
-  </si>
-  <si>
-    <t>23_hongqigongju</t>
-  </si>
-  <si>
-    <t>苗人凤居</t>
-  </si>
-  <si>
-    <t>24_miaorenfengju</t>
-  </si>
-  <si>
-    <t>武道大会</t>
-  </si>
-  <si>
-    <t>25_wudaodahui</t>
-  </si>
-  <si>
-    <t>黑木崖</t>
-  </si>
-  <si>
-    <t>26_heimuya</t>
-  </si>
-  <si>
-    <t>嵩山派</t>
-  </si>
-  <si>
-    <t>27_songshanpai</t>
-  </si>
-  <si>
-    <t>少林寺</t>
-  </si>
-  <si>
-    <t>28_shaolinsi</t>
-  </si>
-  <si>
-    <t>泰山派</t>
-  </si>
-  <si>
-    <t>29_taishanpai</t>
-  </si>
-  <si>
-    <t>平一指居</t>
-  </si>
-  <si>
-    <t>30_pingyizhiju</t>
-  </si>
-  <si>
-    <t>恒山派</t>
-  </si>
-  <si>
-    <t>31_hengshanpai</t>
-  </si>
-  <si>
-    <t>海边小屋</t>
-  </si>
-  <si>
-    <t>32_haibianxiaowu</t>
-  </si>
-  <si>
-    <t>峨嵋派</t>
-  </si>
-  <si>
-    <t>33_emeipai</t>
-  </si>
-  <si>
-    <t>崆峒派</t>
-  </si>
-  <si>
-    <t>34_kongtongpai</t>
-  </si>
-  <si>
-    <t>星宿海</t>
-  </si>
-  <si>
-    <t>35_xingxiuhai</t>
-  </si>
-  <si>
-    <t>青城派</t>
-  </si>
-  <si>
-    <t>36_qingchengpai</t>
-  </si>
-  <si>
-    <t>五毒教</t>
-  </si>
-  <si>
-    <t>37_wudujiao</t>
-  </si>
-  <si>
-    <t>摩天崖</t>
-  </si>
-  <si>
-    <t>38_motianya</t>
-  </si>
-  <si>
-    <t>凌霄城</t>
-  </si>
-  <si>
-    <t>39_lingxiaocheng</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>悦来客栈</t>
-    </r>
-  </si>
-  <si>
-    <t>40_yuelaikezhan</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>神秘山洞</t>
-    </r>
-  </si>
-  <si>
-    <t>41_shandong</t>
-  </si>
-  <si>
-    <t>无量山洞</t>
-  </si>
-  <si>
-    <t>42_wuliangshandong</t>
-  </si>
-  <si>
-    <t>武当派</t>
-  </si>
-  <si>
-    <t>43_wudangpai</t>
-  </si>
-  <si>
-    <t>蝴蝶谷</t>
-  </si>
-  <si>
-    <t>44_hudiegu</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="宋体"/>
+        <rFont val="Microsoft JhengHei UI"/>
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>程英居</t>
+      <t>虾米居</t>
     </r>
-  </si>
-  <si>
-    <t>45_chengyingju</t>
-  </si>
-  <si>
-    <t>金蛇山洞</t>
-  </si>
-  <si>
-    <t>46_jinsheshandong</t>
-  </si>
-  <si>
-    <t>一灯居</t>
-  </si>
-  <si>
-    <t>47_yidengju</t>
-  </si>
-  <si>
-    <t>铁掌山</t>
-  </si>
-  <si>
-    <t>48_tiezhangshan</t>
-  </si>
-  <si>
-    <t>药王庄</t>
-  </si>
-  <si>
-    <t>49_yaowangzhuang</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>阎基居</t>
-    </r>
-  </si>
-  <si>
-    <t>50_yanjiju</t>
-  </si>
-  <si>
-    <t>丐帮</t>
-  </si>
-  <si>
-    <t>51_gaibang</t>
-  </si>
-  <si>
-    <t>燕子坞</t>
-  </si>
-  <si>
-    <t>52_yanziwu</t>
-  </si>
-  <si>
-    <t>擂鼓山</t>
-  </si>
-  <si>
-    <t>53_leigushan</t>
-  </si>
-  <si>
-    <t>薛慕华居</t>
-  </si>
-  <si>
-    <t>54_xuemuhuaju</t>
-  </si>
-  <si>
-    <t>梅庄</t>
-  </si>
-  <si>
-    <t>55_meizhuang</t>
-  </si>
-  <si>
-    <t>Leave:1000,Leave2:82</t>
-  </si>
-  <si>
-    <t>福威镖局</t>
-  </si>
-  <si>
-    <t>56_fuweibiaoju</t>
-  </si>
-  <si>
-    <t>华山派</t>
-  </si>
-  <si>
-    <t>57_huashanpai</t>
-  </si>
-  <si>
-    <t>衡山派</t>
-  </si>
-  <si>
-    <t>58_hengshanpai</t>
-  </si>
-  <si>
-    <t>田伯光居</t>
-  </si>
-  <si>
-    <t>59_tianboguangju</t>
-  </si>
-  <si>
-    <t>龙门客栈</t>
-  </si>
-  <si>
-    <t>60_longmenkezhan</t>
-  </si>
-  <si>
-    <t>高升客栈</t>
-  </si>
-  <si>
-    <t>61_gaoshengkezhan</t>
-  </si>
-  <si>
-    <t>破庙</t>
-  </si>
-  <si>
-    <t>62_pomiao</t>
-  </si>
-  <si>
-    <t>天宁寺</t>
-  </si>
-  <si>
-    <t>63_tianningsi</t>
-  </si>
-  <si>
-    <t>南贤居</t>
-  </si>
-  <si>
-    <t>64_nanxianju</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>唐诗山洞</t>
-    </r>
-  </si>
-  <si>
-    <t>65_shandong</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>冰蚕山洞</t>
-    </r>
-  </si>
-  <si>
-    <t>66_shandong</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>昆仑山洞</t>
-    </r>
-  </si>
-  <si>
-    <t>67_shandong</t>
-  </si>
-  <si>
-    <t>Leave:1000,Leave2:4</t>
-  </si>
-  <si>
-    <t>昆仑派</t>
-  </si>
-  <si>
-    <t>68_kunlunpai</t>
-  </si>
-  <si>
-    <t>白驼山</t>
-  </si>
-  <si>
-    <t>69_baituoshan</t>
-  </si>
-  <si>
-    <t>小虾米居</t>
-  </si>
-  <si>
-    <t>70_xiaoxiamiju</t>
-  </si>
-  <si>
-    <t>START:0</t>
-  </si>
-  <si>
-    <t>神龙教</t>
-  </si>
-  <si>
-    <t>71_shenlongjiao</t>
-  </si>
-  <si>
-    <t>冰火岛</t>
-  </si>
-  <si>
-    <t>72_binghuodao</t>
-  </si>
-  <si>
-    <t>灵蛇岛</t>
-  </si>
-  <si>
-    <t>73_lingshedao</t>
-  </si>
-  <si>
-    <t>侠客岛</t>
-  </si>
-  <si>
-    <t>74_xiakedao</t>
-  </si>
-  <si>
-    <t>桃花岛</t>
-  </si>
-  <si>
-    <t>75_taohuadao</t>
-  </si>
-  <si>
-    <t>霹雳堂</t>
-  </si>
-  <si>
-    <t>76_pilitang</t>
-  </si>
-  <si>
-    <t>Leave:1000,Leave2:83</t>
-  </si>
-  <si>
-    <t>万鳄岛</t>
-  </si>
-  <si>
-    <t>77_wanedao</t>
-  </si>
-  <si>
-    <t>渤泥岛</t>
-  </si>
-  <si>
-    <t>78_bonidao</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鸳鸯山洞</t>
-    </r>
-  </si>
-  <si>
-    <t>79_shandong</t>
-  </si>
-  <si>
-    <t>绝情谷底</t>
-  </si>
-  <si>
-    <t>80_jueqinggudi</t>
-  </si>
-  <si>
-    <t>思过崖</t>
-  </si>
-  <si>
-    <t>81_siguoya</t>
-  </si>
-  <si>
-    <t>梅庄地牢</t>
-  </si>
-  <si>
-    <t>82_meizhuangdilao</t>
-  </si>
-  <si>
-    <t>Leave:55</t>
-  </si>
-  <si>
-    <t>圣堂</t>
-  </si>
-  <si>
-    <t>83_shengtang</t>
-  </si>
-  <si>
-    <t>Leave:76</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>大地图</t>
-    </r>
-  </si>
-  <si>
-    <t>WORLDMAP</t>
-  </si>
-  <si>
-    <t>1000_daditu</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>신룡교</t>
+  </si>
+  <si>
+    <t>빙화도</t>
+  </si>
+  <si>
+    <t>영사도</t>
+  </si>
+  <si>
+    <t>협객도</t>
+  </si>
+  <si>
+    <t>도화도</t>
+  </si>
+  <si>
+    <t>벽력당</t>
+  </si>
+  <si>
+    <t>만악도</t>
+  </si>
+  <si>
+    <t>발니도</t>
+  </si>
+  <si>
+    <t>원앙동굴</t>
+  </si>
+  <si>
+    <t>절정계곡</t>
+  </si>
+  <si>
+    <t>사과애</t>
+  </si>
+  <si>
+    <t>매장 지하감옥</t>
+  </si>
+  <si>
+    <t>성당</t>
+  </si>
+  <si>
+    <t>대지도</t>
+  </si>
+  <si>
+    <t>설모화거처</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>Map</t>
+    <t>성수해</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>LuaConfigGen</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>L_number</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>L_string</t>
+    <t>틈왕동굴</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -808,7 +723,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -860,6 +775,59 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="돋움체"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="KaiTi"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움체"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움체"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft JhengHei UI"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="맑은 고딕 Semilight"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -895,7 +863,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -909,14 +877,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="普通" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="普通 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="普通 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="普通 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -1263,30 +1236,30 @@
   <dimension ref="A1:AU204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="9.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="6" width="9" style="2"/>
-    <col min="7" max="7" width="11.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.08984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.125" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28">
       <c r="A1" s="2" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1332,30 +1305,30 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" s="3" t="s">
-        <v>203</v>
+        <v>118</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>204</v>
+        <v>119</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>204</v>
+        <v>119</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>204</v>
+        <v>119</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>203</v>
+        <v>118</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>203</v>
+        <v>118</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>203</v>
+        <v>118</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>204</v>
+        <v>119</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1378,7 +1351,7 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="12.75">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1404,18 +1377,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="3">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="E5" s="3">
         <v>-1</v>
@@ -1448,18 +1421,18 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
+      <c r="B6" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
@@ -1492,18 +1465,18 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
+      <c r="B7" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3">
         <v>-1</v>
@@ -1536,18 +1509,18 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
+      <c r="B8" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
@@ -1580,18 +1553,18 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
+      <c r="B9" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3">
         <v>8</v>
@@ -1603,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -1626,18 +1599,18 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
+      <c r="B10" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3">
         <v>12</v>
@@ -1649,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -1672,18 +1645,18 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="3">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
+      <c r="B11" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3">
         <v>11</v>
@@ -1716,18 +1689,18 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="3">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>33</v>
+      <c r="B12" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3">
         <v>12</v>
@@ -1739,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1762,18 +1735,18 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="3">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
+      <c r="B13" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3">
         <v>4</v>
@@ -1806,18 +1779,18 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="3">
         <v>9</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>37</v>
+      <c r="B14" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3">
         <v>-1</v>
@@ -1850,18 +1823,18 @@
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="3">
         <v>10</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>39</v>
+      <c r="B15" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3">
         <v>12</v>
@@ -1873,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1896,18 +1869,18 @@
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="3">
         <v>11</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>41</v>
+      <c r="B16" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3">
         <v>10</v>
@@ -1940,18 +1913,18 @@
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28">
       <c r="A17" s="3">
         <v>12</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>43</v>
+      <c r="B17" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E17" s="3">
         <v>-1</v>
@@ -1984,18 +1957,18 @@
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18" s="3">
         <v>13</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
+      <c r="B18" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E18" s="3">
         <v>12</v>
@@ -2028,18 +2001,18 @@
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28">
       <c r="A19" s="3">
         <v>14</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>49</v>
+      <c r="B19" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E19" s="3">
         <v>12</v>
@@ -2051,7 +2024,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -2074,18 +2047,18 @@
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28">
       <c r="A20" s="3">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>52</v>
+      <c r="B20" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E20" s="3">
         <v>12</v>
@@ -2118,18 +2091,18 @@
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28">
       <c r="A21" s="3">
         <v>16</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>55</v>
+      <c r="B21" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3">
         <v>4</v>
@@ -2162,18 +2135,18 @@
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28">
       <c r="A22" s="3">
         <v>17</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>57</v>
+      <c r="B22" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E22" s="3">
         <v>4</v>
@@ -2206,18 +2179,18 @@
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28">
       <c r="A23" s="3">
         <v>18</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>59</v>
+      <c r="B23" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="3">
         <v>12</v>
@@ -2229,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -2252,18 +2225,18 @@
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28">
       <c r="A24" s="3">
         <v>19</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>61</v>
+      <c r="B24" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3">
         <v>22</v>
@@ -2296,18 +2269,18 @@
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28">
       <c r="A25" s="3">
         <v>20</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>63</v>
+      <c r="B25" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E25" s="3">
         <v>13</v>
@@ -2340,18 +2313,18 @@
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28">
       <c r="A26" s="3">
         <v>21</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>65</v>
+      <c r="B26" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3">
         <v>8</v>
@@ -2363,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -2386,18 +2359,18 @@
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28">
       <c r="A27" s="3">
         <v>22</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>68</v>
+      <c r="B27" s="8" t="s">
+        <v>141</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3">
         <v>-1</v>
@@ -2430,18 +2403,18 @@
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28">
       <c r="A28" s="3">
         <v>23</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>70</v>
+      <c r="B28" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" s="3">
         <v>-1</v>
@@ -2474,18 +2447,18 @@
       <c r="AA28" s="3"/>
       <c r="AB28" s="3"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28">
       <c r="A29" s="3">
         <v>24</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>72</v>
+      <c r="B29" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3">
         <v>-1</v>
@@ -2518,18 +2491,18 @@
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28">
       <c r="A30" s="3">
         <v>25</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>74</v>
+      <c r="B30" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E30" s="3">
         <v>15</v>
@@ -2562,18 +2535,18 @@
       <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28">
       <c r="A31" s="3">
         <v>26</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>76</v>
+      <c r="B31" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E31" s="3">
         <v>-1</v>
@@ -2606,18 +2579,18 @@
       <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28">
       <c r="A32" s="3">
         <v>27</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>78</v>
+      <c r="B32" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E32" s="3">
         <v>-1</v>
@@ -2650,18 +2623,18 @@
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28">
       <c r="A33" s="3">
         <v>28</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>80</v>
+      <c r="B33" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3">
         <v>20</v>
@@ -2694,18 +2667,18 @@
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28">
       <c r="A34" s="3">
         <v>29</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>82</v>
+      <c r="B34" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E34" s="3">
         <v>22</v>
@@ -2738,18 +2711,18 @@
       <c r="AA34" s="3"/>
       <c r="AB34" s="3"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28">
       <c r="A35" s="3">
         <v>30</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>84</v>
+      <c r="B35" s="7" t="s">
+        <v>149</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E35" s="3">
         <v>-1</v>
@@ -2782,18 +2755,18 @@
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28">
       <c r="A36" s="3">
         <v>31</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>86</v>
+      <c r="B36" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E36" s="3">
         <v>21</v>
@@ -2826,18 +2799,18 @@
       <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28">
       <c r="A37" s="3">
         <v>32</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>88</v>
+      <c r="B37" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -2870,18 +2843,18 @@
       <c r="AA37" s="3"/>
       <c r="AB37" s="3"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28">
       <c r="A38" s="3">
         <v>33</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>90</v>
+      <c r="B38" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E38" s="3">
         <v>23</v>
@@ -2914,18 +2887,18 @@
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28">
       <c r="A39" s="3">
         <v>34</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>92</v>
+      <c r="B39" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="3">
         <v>-1</v>
@@ -2958,18 +2931,18 @@
       <c r="AA39" s="3"/>
       <c r="AB39" s="3"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28">
       <c r="A40" s="3">
         <v>35</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>94</v>
+      <c r="B40" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" s="3">
         <v>4</v>
@@ -3002,18 +2975,18 @@
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28">
       <c r="A41" s="3">
         <v>36</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>96</v>
+      <c r="B41" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E41" s="3">
         <v>-1</v>
@@ -3046,18 +3019,18 @@
       <c r="AA41" s="3"/>
       <c r="AB41" s="3"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28">
       <c r="A42" s="3">
         <v>37</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>98</v>
+      <c r="B42" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" s="3">
         <v>-1</v>
@@ -3090,18 +3063,18 @@
       <c r="AA42" s="3"/>
       <c r="AB42" s="3"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28">
       <c r="A43" s="3">
         <v>38</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>100</v>
+      <c r="B43" s="7" t="s">
+        <v>156</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E43" s="3">
         <v>-1</v>
@@ -3134,18 +3107,18 @@
       <c r="AA43" s="3"/>
       <c r="AB43" s="3"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28">
       <c r="A44" s="3">
         <v>39</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>102</v>
+      <c r="B44" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" s="3">
         <v>4</v>
@@ -3178,18 +3151,18 @@
       <c r="AA44" s="3"/>
       <c r="AB44" s="3"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28">
       <c r="A45" s="3">
         <v>40</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>104</v>
+      <c r="B45" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3">
         <v>2</v>
@@ -3222,18 +3195,18 @@
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28">
       <c r="A46" s="3">
         <v>41</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>106</v>
+      <c r="B46" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E46" s="3">
         <v>12</v>
@@ -3245,7 +3218,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -3268,18 +3241,18 @@
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28">
       <c r="A47" s="3">
         <v>42</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>108</v>
+      <c r="B47" s="7" t="s">
+        <v>160</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E47" s="3">
         <v>12</v>
@@ -3291,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
@@ -3314,18 +3287,18 @@
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28">
       <c r="A48" s="3">
         <v>43</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>110</v>
+      <c r="B48" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E48" s="3">
         <v>22</v>
@@ -3358,18 +3331,18 @@
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28">
       <c r="A49" s="3">
         <v>44</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>112</v>
+      <c r="B49" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E49" s="3">
         <v>-1</v>
@@ -3402,18 +3375,18 @@
       <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28">
       <c r="A50" s="3">
         <v>45</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>114</v>
+      <c r="B50" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E50" s="3">
         <v>8</v>
@@ -3446,18 +3419,18 @@
       <c r="AA50" s="3"/>
       <c r="AB50" s="3"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28">
       <c r="A51" s="3">
         <v>46</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>116</v>
+      <c r="B51" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E51" s="3">
         <v>12</v>
@@ -3469,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
@@ -3492,18 +3465,18 @@
       <c r="AA51" s="3"/>
       <c r="AB51" s="3"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28">
       <c r="A52" s="3">
         <v>47</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>118</v>
+      <c r="B52" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E52" s="3">
         <v>8</v>
@@ -3536,18 +3509,18 @@
       <c r="AA52" s="3"/>
       <c r="AB52" s="3"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28">
       <c r="A53" s="3">
         <v>48</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>120</v>
+      <c r="B53" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E53" s="3">
         <v>-1</v>
@@ -3580,18 +3553,18 @@
       <c r="AA53" s="3"/>
       <c r="AB53" s="3"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28">
       <c r="A54" s="3">
         <v>49</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>122</v>
+      <c r="B54" s="8" t="s">
+        <v>167</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E54" s="3">
         <v>1</v>
@@ -3624,18 +3597,18 @@
       <c r="AA54" s="3"/>
       <c r="AB54" s="3"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28">
       <c r="A55" s="3">
         <v>50</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>124</v>
+      <c r="B55" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E55" s="3">
         <v>1</v>
@@ -3668,18 +3641,18 @@
       <c r="AA55" s="3"/>
       <c r="AB55" s="3"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28">
       <c r="A56" s="3">
         <v>51</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>126</v>
+      <c r="B56" s="10" t="s">
+        <v>169</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E56" s="3">
         <v>-1</v>
@@ -3712,18 +3685,18 @@
       <c r="AA56" s="3"/>
       <c r="AB56" s="3"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28">
       <c r="A57" s="3">
         <v>52</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>128</v>
+      <c r="B57" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E57" s="3">
         <v>1</v>
@@ -3756,18 +3729,18 @@
       <c r="AA57" s="3"/>
       <c r="AB57" s="3"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28">
       <c r="A58" s="3">
         <v>53</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>130</v>
+      <c r="B58" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E58" s="3">
         <v>-1</v>
@@ -3800,18 +3773,18 @@
       <c r="AA58" s="3"/>
       <c r="AB58" s="3"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28">
       <c r="A59" s="3">
         <v>54</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>132</v>
+      <c r="B59" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E59" s="3">
         <v>-1</v>
@@ -3844,18 +3817,18 @@
       <c r="AA59" s="3"/>
       <c r="AB59" s="3"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28">
       <c r="A60" s="3">
         <v>55</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>134</v>
+      <c r="B60" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="E60" s="3">
         <v>1</v>
@@ -3888,18 +3861,18 @@
       <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28">
       <c r="A61" s="3">
         <v>56</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>137</v>
+      <c r="B61" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E61" s="3">
         <v>9</v>
@@ -3932,18 +3905,18 @@
       <c r="AA61" s="3"/>
       <c r="AB61" s="3"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28">
       <c r="A62" s="3">
         <v>57</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>139</v>
+      <c r="B62" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E62" s="3">
         <v>-1</v>
@@ -3976,18 +3949,18 @@
       <c r="AA62" s="3"/>
       <c r="AB62" s="3"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28">
       <c r="A63" s="3">
         <v>58</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>141</v>
+      <c r="B63" s="7" t="s">
+        <v>175</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E63" s="3">
         <v>-1</v>
@@ -4020,18 +3993,18 @@
       <c r="AA63" s="3"/>
       <c r="AB63" s="3"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28">
       <c r="A64" s="3">
         <v>59</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>143</v>
+      <c r="B64" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E64" s="3">
         <v>-1</v>
@@ -4064,18 +4037,18 @@
       <c r="AA64" s="3"/>
       <c r="AB64" s="3"/>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28">
       <c r="A65" s="3">
         <v>60</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>145</v>
+      <c r="B65" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E65" s="3">
         <v>2</v>
@@ -4108,18 +4081,18 @@
       <c r="AA65" s="3"/>
       <c r="AB65" s="3"/>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28">
       <c r="A66" s="3">
         <v>61</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>147</v>
+      <c r="B66" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>148</v>
+        <v>86</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E66" s="3">
         <v>2</v>
@@ -4152,18 +4125,18 @@
       <c r="AA66" s="3"/>
       <c r="AB66" s="3"/>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28">
       <c r="A67" s="3">
         <v>62</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>149</v>
+      <c r="B67" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E67" s="3">
         <v>-1</v>
@@ -4196,18 +4169,18 @@
       <c r="AA67" s="3"/>
       <c r="AB67" s="3"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28">
       <c r="A68" s="3">
         <v>63</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>151</v>
+      <c r="B68" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E68" s="3">
         <v>-1</v>
@@ -4240,18 +4213,18 @@
       <c r="AA68" s="3"/>
       <c r="AB68" s="3"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28">
       <c r="A69" s="3">
         <v>64</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>153</v>
+      <c r="B69" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E69" s="3">
         <v>11</v>
@@ -4284,18 +4257,18 @@
       <c r="AA69" s="3"/>
       <c r="AB69" s="3"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28">
       <c r="A70" s="3">
         <v>65</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>155</v>
+      <c r="B70" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E70" s="3">
         <v>12</v>
@@ -4307,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
@@ -4330,18 +4303,18 @@
       <c r="AA70" s="3"/>
       <c r="AB70" s="3"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28">
       <c r="A71" s="3">
         <v>66</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>157</v>
+      <c r="B71" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E71" s="3">
         <v>12</v>
@@ -4353,7 +4326,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
@@ -4376,18 +4349,18 @@
       <c r="AA71" s="3"/>
       <c r="AB71" s="3"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28">
       <c r="A72" s="3">
         <v>67</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>159</v>
+      <c r="B72" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>161</v>
+        <v>93</v>
       </c>
       <c r="E72" s="3">
         <v>12</v>
@@ -4399,7 +4372,7 @@
         <v>1</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
@@ -4422,18 +4395,18 @@
       <c r="AA72" s="3"/>
       <c r="AB72" s="3"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28">
       <c r="A73" s="3">
         <v>68</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>162</v>
+      <c r="B73" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>163</v>
+        <v>94</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E73" s="3">
         <v>4</v>
@@ -4466,18 +4439,18 @@
       <c r="AA73" s="3"/>
       <c r="AB73" s="3"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28">
       <c r="A74" s="3">
         <v>69</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>164</v>
+      <c r="B74" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E74" s="3">
         <v>4</v>
@@ -4510,18 +4483,18 @@
       <c r="AA74" s="3"/>
       <c r="AB74" s="3"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28">
       <c r="A75" s="3">
         <v>70</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>166</v>
+      <c r="B75" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>167</v>
+        <v>96</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E75" s="3">
         <v>-1</v>
@@ -4533,7 +4506,7 @@
         <v>0</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
@@ -4556,18 +4529,18 @@
       <c r="AA75" s="3"/>
       <c r="AB75" s="3"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28">
       <c r="A76" s="3">
         <v>71</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>169</v>
+      <c r="B76" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E76" s="3">
         <v>-1</v>
@@ -4600,18 +4573,18 @@
       <c r="AA76" s="3"/>
       <c r="AB76" s="3"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28">
       <c r="A77" s="3">
         <v>72</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>171</v>
+      <c r="B77" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>172</v>
+        <v>99</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E77" s="3">
         <v>12</v>
@@ -4623,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
@@ -4646,18 +4619,18 @@
       <c r="AA77" s="3"/>
       <c r="AB77" s="3"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28">
       <c r="A78" s="3">
         <v>73</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>173</v>
+      <c r="B78" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E78" s="3">
         <v>-1</v>
@@ -4690,18 +4663,18 @@
       <c r="AA78" s="3"/>
       <c r="AB78" s="3"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28">
       <c r="A79" s="3">
         <v>74</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>175</v>
+      <c r="B79" s="10" t="s">
+        <v>190</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>176</v>
+        <v>101</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E79" s="3">
         <v>12</v>
@@ -4734,18 +4707,18 @@
       <c r="AA79" s="3"/>
       <c r="AB79" s="3"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28">
       <c r="A80" s="3">
         <v>75</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>177</v>
+      <c r="B80" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E80" s="3">
         <v>-1</v>
@@ -4778,18 +4751,18 @@
       <c r="AA80" s="3"/>
       <c r="AB80" s="3"/>
     </row>
-    <row r="81" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:47">
       <c r="A81" s="3">
         <v>76</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>179</v>
+      <c r="B81" s="7" t="s">
+        <v>192</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>180</v>
+        <v>103</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="E81" s="3">
         <v>-1</v>
@@ -4822,18 +4795,18 @@
       <c r="AA81" s="3"/>
       <c r="AB81" s="3"/>
     </row>
-    <row r="82" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:47">
       <c r="A82" s="3">
         <v>77</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>182</v>
+      <c r="B82" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E82" s="3">
         <v>-1</v>
@@ -4866,18 +4839,18 @@
       <c r="AA82" s="3"/>
       <c r="AB82" s="3"/>
     </row>
-    <row r="83" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:47">
       <c r="A83" s="3">
         <v>78</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>184</v>
+      <c r="B83" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>185</v>
+        <v>106</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E83" s="3">
         <v>-1</v>
@@ -4910,18 +4883,18 @@
       <c r="AA83" s="3"/>
       <c r="AB83" s="3"/>
     </row>
-    <row r="84" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:47">
       <c r="A84" s="3">
         <v>79</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>186</v>
+      <c r="B84" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E84" s="3">
         <v>12</v>
@@ -4954,18 +4927,18 @@
       <c r="AA84" s="3"/>
       <c r="AB84" s="3"/>
     </row>
-    <row r="85" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:47">
       <c r="A85" s="3">
         <v>80</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>188</v>
+      <c r="B85" s="8" t="s">
+        <v>196</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>189</v>
+        <v>108</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E85" s="3">
         <v>9</v>
@@ -4998,18 +4971,18 @@
       <c r="AA85" s="3"/>
       <c r="AB85" s="3"/>
     </row>
-    <row r="86" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:47">
       <c r="A86" s="3">
         <v>81</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>190</v>
+      <c r="B86" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>191</v>
+        <v>109</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E86" s="3">
         <v>16</v>
@@ -5042,18 +5015,18 @@
       <c r="AA86" s="3"/>
       <c r="AB86" s="3"/>
     </row>
-    <row r="87" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:47">
       <c r="A87" s="3">
         <v>82</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>192</v>
+      <c r="B87" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>193</v>
+        <v>110</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="E87" s="3">
         <v>12</v>
@@ -5086,18 +5059,18 @@
       <c r="AA87" s="3"/>
       <c r="AB87" s="3"/>
     </row>
-    <row r="88" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:47">
       <c r="A88" s="3">
         <v>83</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>195</v>
+      <c r="B88" s="12" t="s">
+        <v>199</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>196</v>
+        <v>112</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>197</v>
+        <v>113</v>
       </c>
       <c r="E88" s="3">
         <v>17</v>
@@ -5109,7 +5082,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
@@ -5132,15 +5105,15 @@
       <c r="AA88" s="3"/>
       <c r="AB88" s="3"/>
     </row>
-    <row r="89" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:47">
       <c r="A89" s="3">
         <v>1000</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>198</v>
+      <c r="B89" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>200</v>
+        <v>115</v>
       </c>
       <c r="D89" s="6">
         <v>-1</v>
@@ -5155,7 +5128,7 @@
         <v>0</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>199</v>
+        <v>114</v>
       </c>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
@@ -5197,7 +5170,7 @@
       <c r="AT89" s="3"/>
       <c r="AU89" s="3"/>
     </row>
-    <row r="90" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:47">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5246,7 +5219,7 @@
       <c r="AT90" s="3"/>
       <c r="AU90" s="3"/>
     </row>
-    <row r="91" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:47">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5295,7 +5268,7 @@
       <c r="AT91" s="3"/>
       <c r="AU91" s="3"/>
     </row>
-    <row r="92" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:47">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5344,7 +5317,7 @@
       <c r="AT92" s="3"/>
       <c r="AU92" s="3"/>
     </row>
-    <row r="93" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:47">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5393,7 +5366,7 @@
       <c r="AT93" s="3"/>
       <c r="AU93" s="3"/>
     </row>
-    <row r="94" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:47">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5442,7 +5415,7 @@
       <c r="AT94" s="3"/>
       <c r="AU94" s="3"/>
     </row>
-    <row r="95" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:47">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5491,7 +5464,7 @@
       <c r="AT95" s="3"/>
       <c r="AU95" s="3"/>
     </row>
-    <row r="96" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:47">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5540,7 +5513,7 @@
       <c r="AT96" s="3"/>
       <c r="AU96" s="3"/>
     </row>
-    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:47">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5589,7 +5562,7 @@
       <c r="AT97" s="3"/>
       <c r="AU97" s="3"/>
     </row>
-    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:47">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5638,7 +5611,7 @@
       <c r="AT98" s="3"/>
       <c r="AU98" s="3"/>
     </row>
-    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:47">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5687,7 +5660,7 @@
       <c r="AT99" s="3"/>
       <c r="AU99" s="3"/>
     </row>
-    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:47">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5736,7 +5709,7 @@
       <c r="AT100" s="3"/>
       <c r="AU100" s="3"/>
     </row>
-    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:47">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5785,7 +5758,7 @@
       <c r="AT101" s="3"/>
       <c r="AU101" s="3"/>
     </row>
-    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:47">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -5834,7 +5807,7 @@
       <c r="AT102" s="3"/>
       <c r="AU102" s="3"/>
     </row>
-    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:47">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5883,7 +5856,7 @@
       <c r="AT103" s="3"/>
       <c r="AU103" s="3"/>
     </row>
-    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:47">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -5932,7 +5905,7 @@
       <c r="AT104" s="3"/>
       <c r="AU104" s="3"/>
     </row>
-    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:47">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5981,7 +5954,7 @@
       <c r="AT105" s="3"/>
       <c r="AU105" s="3"/>
     </row>
-    <row r="106" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:47">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -6030,7 +6003,7 @@
       <c r="AT106" s="3"/>
       <c r="AU106" s="3"/>
     </row>
-    <row r="107" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:47">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -6079,7 +6052,7 @@
       <c r="AT107" s="3"/>
       <c r="AU107" s="3"/>
     </row>
-    <row r="108" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:47">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -6128,7 +6101,7 @@
       <c r="AT108" s="3"/>
       <c r="AU108" s="3"/>
     </row>
-    <row r="109" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:47">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -6177,7 +6150,7 @@
       <c r="AT109" s="3"/>
       <c r="AU109" s="3"/>
     </row>
-    <row r="110" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:47">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -6226,7 +6199,7 @@
       <c r="AT110" s="3"/>
       <c r="AU110" s="3"/>
     </row>
-    <row r="111" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:47">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -6275,7 +6248,7 @@
       <c r="AT111" s="3"/>
       <c r="AU111" s="3"/>
     </row>
-    <row r="112" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:47">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -6324,7 +6297,7 @@
       <c r="AT112" s="3"/>
       <c r="AU112" s="3"/>
     </row>
-    <row r="113" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:47">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -6373,7 +6346,7 @@
       <c r="AT113" s="3"/>
       <c r="AU113" s="3"/>
     </row>
-    <row r="114" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:47">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -6422,7 +6395,7 @@
       <c r="AT114" s="3"/>
       <c r="AU114" s="3"/>
     </row>
-    <row r="115" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:47">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -6471,7 +6444,7 @@
       <c r="AT115" s="3"/>
       <c r="AU115" s="3"/>
     </row>
-    <row r="116" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:47">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -6520,7 +6493,7 @@
       <c r="AT116" s="3"/>
       <c r="AU116" s="3"/>
     </row>
-    <row r="117" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:47">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -6569,7 +6542,7 @@
       <c r="AT117" s="3"/>
       <c r="AU117" s="3"/>
     </row>
-    <row r="118" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:47">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -6618,7 +6591,7 @@
       <c r="AT118" s="3"/>
       <c r="AU118" s="3"/>
     </row>
-    <row r="119" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:47">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -6667,7 +6640,7 @@
       <c r="AT119" s="3"/>
       <c r="AU119" s="3"/>
     </row>
-    <row r="120" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:47">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -6716,7 +6689,7 @@
       <c r="AT120" s="3"/>
       <c r="AU120" s="3"/>
     </row>
-    <row r="121" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:47">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -6765,7 +6738,7 @@
       <c r="AT121" s="3"/>
       <c r="AU121" s="3"/>
     </row>
-    <row r="122" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:47">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -6814,7 +6787,7 @@
       <c r="AT122" s="3"/>
       <c r="AU122" s="3"/>
     </row>
-    <row r="123" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:47">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -6863,7 +6836,7 @@
       <c r="AT123" s="3"/>
       <c r="AU123" s="3"/>
     </row>
-    <row r="124" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:47">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -6912,7 +6885,7 @@
       <c r="AT124" s="3"/>
       <c r="AU124" s="3"/>
     </row>
-    <row r="125" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:47">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -6961,7 +6934,7 @@
       <c r="AT125" s="3"/>
       <c r="AU125" s="3"/>
     </row>
-    <row r="126" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:47">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -7010,7 +6983,7 @@
       <c r="AT126" s="3"/>
       <c r="AU126" s="3"/>
     </row>
-    <row r="127" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:47">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -7059,7 +7032,7 @@
       <c r="AT127" s="3"/>
       <c r="AU127" s="3"/>
     </row>
-    <row r="128" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:47">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -7108,7 +7081,7 @@
       <c r="AT128" s="3"/>
       <c r="AU128" s="3"/>
     </row>
-    <row r="129" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:47">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -7157,7 +7130,7 @@
       <c r="AT129" s="3"/>
       <c r="AU129" s="3"/>
     </row>
-    <row r="130" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:47">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -7206,7 +7179,7 @@
       <c r="AT130" s="3"/>
       <c r="AU130" s="3"/>
     </row>
-    <row r="131" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:47">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -7255,7 +7228,7 @@
       <c r="AT131" s="3"/>
       <c r="AU131" s="3"/>
     </row>
-    <row r="132" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:47">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -7304,7 +7277,7 @@
       <c r="AT132" s="3"/>
       <c r="AU132" s="3"/>
     </row>
-    <row r="133" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:47">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -7353,7 +7326,7 @@
       <c r="AT133" s="3"/>
       <c r="AU133" s="3"/>
     </row>
-    <row r="134" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:47">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -7402,7 +7375,7 @@
       <c r="AT134" s="3"/>
       <c r="AU134" s="3"/>
     </row>
-    <row r="135" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:47">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -7451,7 +7424,7 @@
       <c r="AT135" s="3"/>
       <c r="AU135" s="3"/>
     </row>
-    <row r="136" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:47">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -7500,7 +7473,7 @@
       <c r="AT136" s="3"/>
       <c r="AU136" s="3"/>
     </row>
-    <row r="137" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:47">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -7549,7 +7522,7 @@
       <c r="AT137" s="3"/>
       <c r="AU137" s="3"/>
     </row>
-    <row r="138" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:47">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -7598,7 +7571,7 @@
       <c r="AT138" s="3"/>
       <c r="AU138" s="3"/>
     </row>
-    <row r="139" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:47">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -7647,7 +7620,7 @@
       <c r="AT139" s="3"/>
       <c r="AU139" s="3"/>
     </row>
-    <row r="140" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:47">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -7696,7 +7669,7 @@
       <c r="AT140" s="3"/>
       <c r="AU140" s="3"/>
     </row>
-    <row r="141" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:47">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -7745,7 +7718,7 @@
       <c r="AT141" s="3"/>
       <c r="AU141" s="3"/>
     </row>
-    <row r="142" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:47">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -7794,7 +7767,7 @@
       <c r="AT142" s="3"/>
       <c r="AU142" s="3"/>
     </row>
-    <row r="143" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:47">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -7843,7 +7816,7 @@
       <c r="AT143" s="3"/>
       <c r="AU143" s="3"/>
     </row>
-    <row r="144" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:47">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -7892,7 +7865,7 @@
       <c r="AT144" s="3"/>
       <c r="AU144" s="3"/>
     </row>
-    <row r="145" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:47">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -7941,7 +7914,7 @@
       <c r="AT145" s="3"/>
       <c r="AU145" s="3"/>
     </row>
-    <row r="146" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:47">
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -7990,7 +7963,7 @@
       <c r="AT146" s="3"/>
       <c r="AU146" s="3"/>
     </row>
-    <row r="147" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:47">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -8039,7 +8012,7 @@
       <c r="AT147" s="3"/>
       <c r="AU147" s="3"/>
     </row>
-    <row r="148" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:47">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -8088,7 +8061,7 @@
       <c r="AT148" s="3"/>
       <c r="AU148" s="3"/>
     </row>
-    <row r="149" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:47">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -8137,7 +8110,7 @@
       <c r="AT149" s="3"/>
       <c r="AU149" s="3"/>
     </row>
-    <row r="150" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:47">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -8186,7 +8159,7 @@
       <c r="AT150" s="3"/>
       <c r="AU150" s="3"/>
     </row>
-    <row r="151" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:47">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -8235,7 +8208,7 @@
       <c r="AT151" s="3"/>
       <c r="AU151" s="3"/>
     </row>
-    <row r="152" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:47">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -8284,7 +8257,7 @@
       <c r="AT152" s="3"/>
       <c r="AU152" s="3"/>
     </row>
-    <row r="153" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:47">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -8333,7 +8306,7 @@
       <c r="AT153" s="3"/>
       <c r="AU153" s="3"/>
     </row>
-    <row r="154" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:47">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -8382,7 +8355,7 @@
       <c r="AT154" s="3"/>
       <c r="AU154" s="3"/>
     </row>
-    <row r="155" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:47">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -8431,7 +8404,7 @@
       <c r="AT155" s="3"/>
       <c r="AU155" s="3"/>
     </row>
-    <row r="156" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:47">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -8480,7 +8453,7 @@
       <c r="AT156" s="3"/>
       <c r="AU156" s="3"/>
     </row>
-    <row r="157" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:47">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
@@ -8529,7 +8502,7 @@
       <c r="AT157" s="3"/>
       <c r="AU157" s="3"/>
     </row>
-    <row r="158" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:47">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -8578,7 +8551,7 @@
       <c r="AT158" s="3"/>
       <c r="AU158" s="3"/>
     </row>
-    <row r="159" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:47">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -8627,7 +8600,7 @@
       <c r="AT159" s="3"/>
       <c r="AU159" s="3"/>
     </row>
-    <row r="160" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:47">
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -8676,7 +8649,7 @@
       <c r="AT160" s="3"/>
       <c r="AU160" s="3"/>
     </row>
-    <row r="161" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:47">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -8725,7 +8698,7 @@
       <c r="AT161" s="3"/>
       <c r="AU161" s="3"/>
     </row>
-    <row r="162" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:47">
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
@@ -8774,7 +8747,7 @@
       <c r="AT162" s="3"/>
       <c r="AU162" s="3"/>
     </row>
-    <row r="163" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:47">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -8823,7 +8796,7 @@
       <c r="AT163" s="3"/>
       <c r="AU163" s="3"/>
     </row>
-    <row r="164" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:47">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
@@ -8872,7 +8845,7 @@
       <c r="AT164" s="3"/>
       <c r="AU164" s="3"/>
     </row>
-    <row r="165" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:47">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -8921,7 +8894,7 @@
       <c r="AT165" s="3"/>
       <c r="AU165" s="3"/>
     </row>
-    <row r="166" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:47">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -8970,7 +8943,7 @@
       <c r="AT166" s="3"/>
       <c r="AU166" s="3"/>
     </row>
-    <row r="167" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:47">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -9019,7 +8992,7 @@
       <c r="AT167" s="3"/>
       <c r="AU167" s="3"/>
     </row>
-    <row r="168" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:47">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -9068,7 +9041,7 @@
       <c r="AT168" s="3"/>
       <c r="AU168" s="3"/>
     </row>
-    <row r="169" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:47">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
@@ -9117,7 +9090,7 @@
       <c r="AT169" s="3"/>
       <c r="AU169" s="3"/>
     </row>
-    <row r="170" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:47">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
@@ -9166,7 +9139,7 @@
       <c r="AT170" s="3"/>
       <c r="AU170" s="3"/>
     </row>
-    <row r="171" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:47">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
@@ -9215,7 +9188,7 @@
       <c r="AT171" s="3"/>
       <c r="AU171" s="3"/>
     </row>
-    <row r="172" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:47">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
@@ -9264,7 +9237,7 @@
       <c r="AT172" s="3"/>
       <c r="AU172" s="3"/>
     </row>
-    <row r="173" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:47">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
@@ -9313,7 +9286,7 @@
       <c r="AT173" s="3"/>
       <c r="AU173" s="3"/>
     </row>
-    <row r="174" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:47">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
@@ -9362,7 +9335,7 @@
       <c r="AT174" s="3"/>
       <c r="AU174" s="3"/>
     </row>
-    <row r="175" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:47">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
@@ -9411,7 +9384,7 @@
       <c r="AT175" s="3"/>
       <c r="AU175" s="3"/>
     </row>
-    <row r="176" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:47">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
@@ -9460,7 +9433,7 @@
       <c r="AT176" s="3"/>
       <c r="AU176" s="3"/>
     </row>
-    <row r="177" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:47">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
@@ -9509,7 +9482,7 @@
       <c r="AT177" s="3"/>
       <c r="AU177" s="3"/>
     </row>
-    <row r="178" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:47">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
@@ -9558,7 +9531,7 @@
       <c r="AT178" s="3"/>
       <c r="AU178" s="3"/>
     </row>
-    <row r="179" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:47">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
@@ -9607,7 +9580,7 @@
       <c r="AT179" s="3"/>
       <c r="AU179" s="3"/>
     </row>
-    <row r="180" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:47">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
@@ -9656,7 +9629,7 @@
       <c r="AT180" s="3"/>
       <c r="AU180" s="3"/>
     </row>
-    <row r="181" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:47">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
@@ -9705,7 +9678,7 @@
       <c r="AT181" s="3"/>
       <c r="AU181" s="3"/>
     </row>
-    <row r="182" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:47">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
@@ -9754,7 +9727,7 @@
       <c r="AT182" s="3"/>
       <c r="AU182" s="3"/>
     </row>
-    <row r="183" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:47">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
@@ -9803,7 +9776,7 @@
       <c r="AT183" s="3"/>
       <c r="AU183" s="3"/>
     </row>
-    <row r="184" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:47">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
@@ -9852,7 +9825,7 @@
       <c r="AT184" s="3"/>
       <c r="AU184" s="3"/>
     </row>
-    <row r="185" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:47">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
@@ -9901,7 +9874,7 @@
       <c r="AT185" s="3"/>
       <c r="AU185" s="3"/>
     </row>
-    <row r="186" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:47">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
@@ -9950,7 +9923,7 @@
       <c r="AT186" s="3"/>
       <c r="AU186" s="3"/>
     </row>
-    <row r="187" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:47">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
@@ -9999,7 +9972,7 @@
       <c r="AT187" s="3"/>
       <c r="AU187" s="3"/>
     </row>
-    <row r="188" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:47">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
@@ -10048,7 +10021,7 @@
       <c r="AT188" s="3"/>
       <c r="AU188" s="3"/>
     </row>
-    <row r="189" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:47">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
@@ -10097,7 +10070,7 @@
       <c r="AT189" s="3"/>
       <c r="AU189" s="3"/>
     </row>
-    <row r="190" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:47">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
@@ -10146,7 +10119,7 @@
       <c r="AT190" s="3"/>
       <c r="AU190" s="3"/>
     </row>
-    <row r="191" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:47">
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
@@ -10195,7 +10168,7 @@
       <c r="AT191" s="3"/>
       <c r="AU191" s="3"/>
     </row>
-    <row r="192" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:47">
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
@@ -10244,7 +10217,7 @@
       <c r="AT192" s="3"/>
       <c r="AU192" s="3"/>
     </row>
-    <row r="193" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:47">
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
@@ -10293,7 +10266,7 @@
       <c r="AT193" s="3"/>
       <c r="AU193" s="3"/>
     </row>
-    <row r="194" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:47">
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
@@ -10342,7 +10315,7 @@
       <c r="AT194" s="3"/>
       <c r="AU194" s="3"/>
     </row>
-    <row r="195" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:47">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
@@ -10391,7 +10364,7 @@
       <c r="AT195" s="3"/>
       <c r="AU195" s="3"/>
     </row>
-    <row r="196" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:47">
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
@@ -10440,7 +10413,7 @@
       <c r="AT196" s="3"/>
       <c r="AU196" s="3"/>
     </row>
-    <row r="197" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:47">
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
@@ -10489,7 +10462,7 @@
       <c r="AT197" s="3"/>
       <c r="AU197" s="3"/>
     </row>
-    <row r="198" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:47">
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
@@ -10538,7 +10511,7 @@
       <c r="AT198" s="3"/>
       <c r="AU198" s="3"/>
     </row>
-    <row r="199" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:47">
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
@@ -10587,7 +10560,7 @@
       <c r="AT199" s="3"/>
       <c r="AU199" s="3"/>
     </row>
-    <row r="200" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:47">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
@@ -10636,7 +10609,7 @@
       <c r="AT200" s="3"/>
       <c r="AU200" s="3"/>
     </row>
-    <row r="201" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:47">
       <c r="A201" s="3"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
@@ -10685,7 +10658,7 @@
       <c r="AT201" s="3"/>
       <c r="AU201" s="3"/>
     </row>
-    <row r="202" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:47">
       <c r="A202" s="3"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
@@ -10734,7 +10707,7 @@
       <c r="AT202" s="3"/>
       <c r="AU202" s="3"/>
     </row>
-    <row r="203" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:47">
       <c r="A203" s="3"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
@@ -10783,7 +10756,7 @@
       <c r="AT203" s="3"/>
       <c r="AU203" s="3"/>
     </row>
-    <row r="204" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:47">
       <c r="A204" s="3"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>

</xml_diff>